<commit_message>
Modified the test data
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,9 +27,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Hdfc</t>
-  </si>
-  <si>
     <t>IDFC</t>
   </si>
   <si>
@@ -43,9 +39,6 @@
     <t>Axis</t>
   </si>
   <si>
-    <t>Hdfc Bank</t>
-  </si>
-  <si>
     <t>IDFC Bank</t>
   </si>
   <si>
@@ -56,6 +49,12 @@
   </si>
   <si>
     <t>Axis Bank</t>
+  </si>
+  <si>
+    <t>Canara</t>
+  </si>
+  <si>
+    <t>Canara Bank</t>
   </si>
 </sst>
 </file>
@@ -376,7 +375,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -394,42 +393,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>